<commit_message>
Now all data imports work again
</commit_message>
<xml_diff>
--- a/templates/building_template.xlsx
+++ b/templates/building_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suraj/Documents/Haaga-Helia/Software Project/siba-fe/src/tempates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitHubRepos_4\Siba23k\Siba_be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5154D03-E4F4-9D44-A10C-EDA1BAB7D245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE2274F-61AB-448E-B571-CC2290C8F8C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{4C06AEAF-13B2-B045-AEA5-306F0C879648}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -426,9 +415,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.58203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -444,7 +436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -452,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>

</xml_diff>